<commit_message>
First pass stores and routes for Odisha_Food, plus transitmatrix.csv
</commit_message>
<xml_diff>
--- a/HERMES2/master_data/Odisha_Food/hectares_by_tehsil.xlsx
+++ b/HERMES2/master_data/Odisha_Food/hectares_by_tehsil.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Provenance" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="59">
   <si>
     <t xml:space="preserve">The data of hectares under cultivation for potatoes in each tehsil is extracted by hand from Box/Hermes Food/Data_Conventional/Data_1_Farms and Potato Production/AgCensus_PotatoAreaBySize, with some updates to place names, on 7/26/2016</t>
   </si>
@@ -168,6 +168,36 @@
   </si>
   <si>
     <t xml:space="preserve">Muribahal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khurda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balianta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balipatana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banapur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begunia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhubaneswar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolagarh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chilika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jatani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tangi</t>
   </si>
 </sst>
 </file>
@@ -182,6 +212,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -265,13 +296,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,15 +331,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="810" topLeftCell="A23" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,10 +1072,180 @@
         <v>83.0125827</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>20.3068913</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>85.8826348</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>20.2019765</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>85.9513664</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>19.77496</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>85.1473472</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>19.83368</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>85.3244626</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>20.3010311</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>85.750413</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>20.1747906</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>85.2665969</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>19.6671344</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>85.3763267</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>20.1612971</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>85.6782954</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>20.1796469</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>85.6243513</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>19.925275</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>85.3838936</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>